<commit_message>
Se agrega semillerio, se agrega notebook con optimizacion bayesiana y se pone parametrizable el periodo de los productos a discontinuar
</commit_message>
<xml_diff>
--- a/docs/EstrategiaEntrenamiento.xlsx
+++ b/docs/EstrategiaEntrenamiento.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_MCD\_Labo3\code\labo3_empresa3\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBEB970D-70EF-418A-B237-C3DB609B6171}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B93911F-506C-445E-9C06-908F293F0041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{85493C32-C117-4849-B6F2-A1657B042679}"/>
+    <workbookView minimized="1" xWindow="26715" yWindow="2535" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{85493C32-C117-4849-B6F2-A1657B042679}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="17">
   <si>
     <t>Opción 1</t>
   </si>
@@ -85,6 +85,9 @@
   </si>
   <si>
     <t>Final Train</t>
+  </si>
+  <si>
+    <t>Opción 3</t>
   </si>
 </sst>
 </file>
@@ -183,6 +186,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -201,7 +205,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,10 +539,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C3" s="3">
@@ -587,53 +590,53 @@
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+      <c r="C4" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="N5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="7"/>
-      <c r="C6" s="6" t="s">
+      <c r="A6" s="8"/>
+      <c r="C6" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
+      <c r="G6" s="7"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="7"/>
+      <c r="J6" s="7"/>
+      <c r="K6" s="7"/>
+      <c r="L6" s="7"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
       <c r="P6" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="1"/>
@@ -643,18 +646,18 @@
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="8"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
       <c r="G9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
+      <c r="A10" s="8"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8" t="s">
+      <c r="A11" s="8"/>
+      <c r="B11" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C11" s="1"/>
@@ -665,18 +668,18 @@
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="8"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="9"/>
       <c r="H12" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
+      <c r="A13" s="8"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="8" t="s">
+      <c r="A14" s="8"/>
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C14" s="1"/>
@@ -688,18 +691,18 @@
       <c r="G14" s="1"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="9"/>
       <c r="I15" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
+      <c r="A16" s="8"/>
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C17" s="1"/>
@@ -712,68 +715,68 @@
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
       <c r="J18" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="8"/>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
+      <c r="A20" s="8"/>
       <c r="K20" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
+      <c r="A21" s="8"/>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="8" t="s">
+      <c r="A22" s="8"/>
+      <c r="B22" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
+      <c r="C22" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="11"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="11"/>
+      <c r="G22" s="11"/>
+      <c r="H22" s="11"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="11"/>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11"/>
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="9"/>
       <c r="N23" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
+      <c r="A24" s="8"/>
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
-      <c r="C25" s="6" t="s">
+      <c r="A25" s="8"/>
+      <c r="C25" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="6"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="6"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="6"/>
-      <c r="J25" s="6"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="6"/>
-      <c r="M25" s="6"/>
-      <c r="N25" s="6"/>
+      <c r="D25" s="7"/>
+      <c r="E25" s="7"/>
+      <c r="F25" s="7"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
       <c r="P25" s="4" t="s">
         <v>11</v>
       </c>
@@ -802,23 +805,23 @@
   <dimension ref="A1:P34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="P5" sqref="P5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9"/>
+      <c r="B1" s="10"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="C2" s="3">
-        <v>201801</v>
-      </c>
-      <c r="D2" s="3">
-        <v>201802</v>
+        <v>201701</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="E2" s="3">
         <v>201803</v>
@@ -858,7 +861,7 @@
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -877,16 +880,16 @@
       <c r="N3" s="1"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A4" s="7"/>
+      <c r="A4" s="8"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A5" s="7"/>
+      <c r="A5" s="8"/>
       <c r="P5" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -903,61 +906,61 @@
       <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
+      <c r="A8" s="8"/>
       <c r="N8" s="5" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
+      <c r="A9" s="8"/>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="C10" s="12" t="s">
+      <c r="A10" s="8"/>
+      <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="12"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="12"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A11" s="7"/>
+      <c r="A11" s="8"/>
       <c r="P11" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
+      <c r="A12" s="8"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D14" s="11"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="11"/>
-      <c r="J14" s="11"/>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11"/>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
+      <c r="D14" s="12"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="12"/>
+      <c r="I14" s="12"/>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="12"/>
+      <c r="N14" s="12"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B17" s="8" t="s">
+      <c r="A17" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17" s="9" t="s">
         <v>4</v>
       </c>
       <c r="C17" s="1"/>
@@ -967,18 +970,18 @@
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="9"/>
       <c r="G18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="7"/>
+      <c r="A19" s="8"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="8" t="s">
+      <c r="A20" s="8"/>
+      <c r="B20" s="9" t="s">
         <v>6</v>
       </c>
       <c r="C20" s="1"/>
@@ -989,18 +992,18 @@
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="8"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="9"/>
       <c r="H21" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
+      <c r="A22" s="8"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="8" t="s">
+      <c r="A23" s="8"/>
+      <c r="B23" s="9" t="s">
         <v>7</v>
       </c>
       <c r="C23" s="1"/>
@@ -1012,18 +1015,18 @@
       <c r="G23" s="1"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="8"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="9"/>
       <c r="I24" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="7"/>
+      <c r="A25" s="8"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" s="7"/>
-      <c r="B26" s="8" t="s">
+      <c r="A26" s="8"/>
+      <c r="B26" s="9" t="s">
         <v>8</v>
       </c>
       <c r="C26" s="1"/>
@@ -1036,79 +1039,74 @@
       <c r="H26" s="1"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" s="7"/>
-      <c r="B27" s="8"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
       <c r="J27" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" s="7"/>
+      <c r="A28" s="8"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" s="7"/>
+      <c r="A29" s="8"/>
       <c r="K29" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" s="7"/>
+      <c r="A30" s="8"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" s="7"/>
-      <c r="B31" s="8" t="s">
+      <c r="A31" s="8"/>
+      <c r="B31" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="10"/>
-      <c r="G31" s="10"/>
-      <c r="H31" s="10"/>
-      <c r="I31" s="10"/>
-      <c r="J31" s="10"/>
-      <c r="K31" s="10"/>
-      <c r="L31" s="10"/>
+      <c r="C31" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" s="11"/>
+      <c r="E31" s="11"/>
+      <c r="F31" s="11"/>
+      <c r="G31" s="11"/>
+      <c r="H31" s="11"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="11"/>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A32" s="7"/>
-      <c r="B32" s="8"/>
+      <c r="A32" s="8"/>
+      <c r="B32" s="9"/>
       <c r="N32" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A33" s="7"/>
+      <c r="A33" s="8"/>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A34" s="7"/>
-      <c r="C34" s="6" t="s">
+      <c r="A34" s="8"/>
+      <c r="C34" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="6"/>
-      <c r="E34" s="6"/>
-      <c r="F34" s="6"/>
-      <c r="G34" s="6"/>
-      <c r="H34" s="6"/>
-      <c r="I34" s="6"/>
-      <c r="J34" s="6"/>
-      <c r="K34" s="6"/>
-      <c r="L34" s="6"/>
-      <c r="M34" s="6"/>
-      <c r="N34" s="6"/>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="7"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="7"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
       <c r="P34" s="4" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A3:A5"/>
-    <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A7:A12"/>
-    <mergeCell ref="C14:N14"/>
-    <mergeCell ref="C31:L31"/>
     <mergeCell ref="C34:N34"/>
     <mergeCell ref="A17:A34"/>
     <mergeCell ref="B17:B18"/>
@@ -1116,6 +1114,11 @@
     <mergeCell ref="B23:B24"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B31:B32"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A7:A12"/>
+    <mergeCell ref="C14:N14"/>
+    <mergeCell ref="C31:L31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>